<commit_message>
take out lignite from ets
</commit_message>
<xml_diff>
--- a/InputData/elec/BECF/BAU Expected Capacity Factors.xlsx
+++ b/InputData/elec/BECF/BAU Expected Capacity Factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Canada\canada-eps\InputData\elec\BECF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDA6CE7-8692-4F3D-B8CB-42C7E0D47643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714E1896-05D7-4162-A380-505FDDA63F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3593,7 +3593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -41018,8 +41018,8 @@
   </sheetPr>
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:AG17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41217,7 +41217,7 @@
         <v>0.64</v>
       </c>
       <c r="D2" s="28">
-        <f t="shared" ref="D2:AJ10" si="1">C2</f>
+        <f t="shared" ref="D2:AJ9" si="1">C2</f>
         <v>0.64</v>
       </c>
       <c r="E2" s="28">
@@ -41359,7 +41359,7 @@
         <v>0.13560000000000003</v>
       </c>
       <c r="C3" s="28">
-        <f t="shared" ref="C3:R14" si="2">B3</f>
+        <f t="shared" ref="C3:R12" si="2">B3</f>
         <v>0.13560000000000003</v>
       </c>
       <c r="D3" s="28">
@@ -42751,112 +42751,109 @@
         <v>lignite</v>
       </c>
       <c r="B13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="C13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="D13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="E13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="F13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="G13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="H13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="I13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="J13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="K13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="L13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="M13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="N13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="O13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="P13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="Q13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="R13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="S13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="T13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="U13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="V13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="W13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="X13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="Y13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="Z13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="AA13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="AB13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="AC13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="AD13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="AE13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="AF13">
-        <v>0.376</v>
+        <v>1E-3</v>
       </c>
       <c r="AG13">
-        <v>0.376</v>
-      </c>
-      <c r="AH13" s="28">
-        <f t="shared" si="3"/>
-        <v>0.376</v>
-      </c>
-      <c r="AI13" s="28">
-        <f t="shared" si="3"/>
-        <v>0.376</v>
-      </c>
-      <c r="AJ13" s="28">
-        <f t="shared" si="3"/>
-        <v>0.376</v>
+        <v>1E-3</v>
+      </c>
+      <c r="AH13">
+        <v>1E-3</v>
+      </c>
+      <c r="AI13">
+        <v>1E-3</v>
+      </c>
+      <c r="AJ13">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -45727,7 +45724,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47524,143 +47521,143 @@
       </c>
       <c r="B13" s="28">
         <f>'BECF-pre-ret'!B13*About!B$36</f>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="C13" s="28">
         <f t="shared" si="2"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="D13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="E13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="F13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="G13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="H13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="I13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="J13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="K13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="L13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="M13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="N13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="O13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="P13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="Q13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="R13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="S13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="T13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="U13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="V13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="W13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="X13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="Y13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="Z13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AA13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AB13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AC13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AD13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AE13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AF13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AG13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AH13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AI13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="AJ13" s="28">
         <f t="shared" si="3"/>
-        <v>0.41360000000000002</v>
+        <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -48253,32 +48250,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </of2ed5e60f3c4f8984f283882cb94320>
-    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ff7c4ad8664a4671b57370e258acad6a>
-    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l787e5950a9249679d0130235a9a791b>
-    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6681120aa8fa62dd7a0beb503524cb55">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b98e8ac0331400a99b3dbea3ee620024" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
@@ -48524,25 +48495,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21BE083A-8560-4254-BAB6-CA854611691B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86209414-7AAC-4756-A165-17A53274AF22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </of2ed5e60f3c4f8984f283882cb94320>
+    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ff7c4ad8664a4671b57370e258acad6a>
+    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l787e5950a9249679d0130235a9a791b>
+    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEF58C0D-2D7D-46C7-93E5-4B8A971FE8DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -48560,4 +48539,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86209414-7AAC-4756-A165-17A53274AF22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21BE083A-8560-4254-BAB6-CA854611691B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>